<commit_message>
Prepare model to export with m2cgen
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi.borriello2\Desktop\Tirocinio\Tiny-MachineLearning\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95E6D40-5AEE-4B35-9CA7-9699DF707DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C004C4-D38B-49DB-A928-2D942B7B886A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4369CB72-3CB2-48AE-831B-B67D7B2D2361}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Data</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Sklearn doc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Studio XGB </t>
   </si>
 </sst>
 </file>
@@ -172,16 +175,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -212,10 +215,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{46220553-AC31-43EC-A4E9-DA82EE6C8576}" name="Tabella2" displayName="Tabella2" ref="B2:E20" totalsRowCount="1" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="B2:E19" xr:uid="{46220553-AC31-43EC-A4E9-DA82EE6C8576}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1B096FAB-3866-401A-9AF0-3E9E6BC91087}" name="Data" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{DAB87FCA-D670-4C72-AB2E-3B17BA037396}" name="Ore" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{789F7B6F-7B08-42E9-8AE2-354812F8EF32}" name="Task" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{25867127-5B90-4E64-876B-E1FF828811C7}" name="Fonti utilizzate" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{1B096FAB-3866-401A-9AF0-3E9E6BC91087}" name="Data" dataDxfId="6" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{DAB87FCA-D670-4C72-AB2E-3B17BA037396}" name="Ore" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{789F7B6F-7B08-42E9-8AE2-354812F8EF32}" name="Task" dataDxfId="4" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{25867127-5B90-4E64-876B-E1FF828811C7}" name="Fonti utilizzate" dataDxfId="3" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -521,7 +524,7 @@
   <dimension ref="B1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -535,7 +538,7 @@
     <row r="1" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C1" s="6">
         <f>C3+C4+C5+C6+C7+C8+C9+C11+C10+C12+C13+C14+C15+C16+C18+C17+C19</f>
-        <v>31.5</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
@@ -666,16 +669,24 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="B11" s="4">
+        <v>44605</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>

</xml_diff>

<commit_message>
start evaluate memory occupation
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi.borriello2\Desktop\Tirocinio\Tiny-MachineLearning\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5392E5EF-24E9-48AB-A149-F1D579270B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDB32AC-A017-4418-9A2E-D9EEC321EF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4369CB72-3CB2-48AE-831B-B67D7B2D2361}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Data</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Cross Validation e Model Compar.</t>
+  </si>
+  <si>
+    <t>Model C. e test dei modelli su AD</t>
+  </si>
+  <si>
+    <t>Studio memoria e Inferenza</t>
   </si>
 </sst>
 </file>
@@ -533,21 +539,21 @@
   <dimension ref="B1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13.81640625" customWidth="1"/>
     <col min="3" max="3" width="13.90625" customWidth="1"/>
-    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="4" max="4" width="55.26953125" customWidth="1"/>
     <col min="5" max="5" width="46.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C1" s="6">
         <f>C3+C4+C5+C6+C7+C8+C9+C11+C10+C12+C13+C14+C15+C16+C18+C17+C19</f>
-        <v>40.5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
@@ -720,15 +726,27 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="B14" s="4">
+        <v>44609</v>
+      </c>
+      <c r="C14" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="B15" s="4">
+        <v>44611</v>
+      </c>
+      <c r="C15" s="3">
+        <v>6</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
finish Color model Comparison
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi.borriello2\Desktop\Tirocinio\Tiny-MachineLearning\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDB32AC-A017-4418-9A2E-D9EEC321EF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EEAA55-8347-4F3B-B239-613B174A88B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4369CB72-3CB2-48AE-831B-B67D7B2D2361}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Data</t>
   </si>
@@ -100,13 +100,28 @@
   </si>
   <si>
     <t>Studio memoria e Inferenza</t>
+  </si>
+  <si>
+    <t>test vari</t>
+  </si>
+  <si>
+    <t>studio elettronica arduino</t>
+  </si>
+  <si>
+    <t>test perf su ard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ricerca Paper </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google Scholar / </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,13 +145,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -162,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -179,6 +225,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -227,8 +285,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{46220553-AC31-43EC-A4E9-DA82EE6C8576}" name="Tabella2" displayName="Tabella2" ref="B2:E20" totalsRowCount="1" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="B2:E19" xr:uid="{46220553-AC31-43EC-A4E9-DA82EE6C8576}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{46220553-AC31-43EC-A4E9-DA82EE6C8576}" name="Tabella2" displayName="Tabella2" ref="B2:E21" totalsRowCount="1" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="B2:E20" xr:uid="{46220553-AC31-43EC-A4E9-DA82EE6C8576}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{1B096FAB-3866-401A-9AF0-3E9E6BC91087}" name="Data" dataDxfId="6" totalsRowDxfId="2"/>
     <tableColumn id="2" xr3:uid="{DAB87FCA-D670-4C72-AB2E-3B17BA037396}" name="Ore" dataDxfId="5"/>
@@ -536,37 +594,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC1F251-2E00-4C93-80E5-7B7C0B1560BE}">
-  <dimension ref="B1:I20"/>
+  <dimension ref="B1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13.81640625" customWidth="1"/>
     <col min="3" max="3" width="13.90625" customWidth="1"/>
-    <col min="4" max="4" width="55.26953125" customWidth="1"/>
-    <col min="5" max="5" width="46.26953125" customWidth="1"/>
+    <col min="4" max="4" width="64.81640625" customWidth="1"/>
+    <col min="5" max="5" width="56.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C1" s="6">
-        <f>C3+C4+C5+C6+C7+C8+C9+C11+C10+C12+C13+C14+C15+C16+C18+C17+C19</f>
-        <v>51</v>
+        <f>C3+C4+C5+C6+C7+C8+C9+C11+C10+C12+C13+C14+C15+C16+C18+C17+C19+C20++Tabella2[[#Totals],[Ore]]+C22+C23+C24+C25+C26+C28+C27+C29</f>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="11" t="s">
         <v>3</v>
       </c>
     </row>
@@ -750,33 +808,71 @@
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="B16" s="4">
+        <v>44612</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="B17" s="4">
+        <v>44613</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="B18" s="4">
+        <v>44614</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="B19" s="4">
+        <v>44615</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="B20" s="4">
+        <v>44616</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding samples and test all the test-set
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi.borriello2\Desktop\Tirocinio\Tiny-MachineLearning\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9090779A-4CDE-4235-AEB9-451D71970889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FAA21C-14E4-45E8-AB8D-5C4058E8DE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4369CB72-3CB2-48AE-831B-B67D7B2D2361}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Data</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Test raddoppiando valori</t>
+  </si>
+  <si>
+    <t>Call e check librerie</t>
   </si>
 </sst>
 </file>
@@ -612,7 +615,7 @@
   <dimension ref="B1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,7 +629,7 @@
     <row r="1" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C1" s="6">
         <f>C3+C4+C5+C6+C7+C8+C9+C11+C10+C12+C13+C14+C15+C16+C18+C17+C19+C20++Tabella2[[#Totals],[Ore]]+C22+C23+C24+C25+C26+C29+C27+C30+C21</f>
-        <v>73.5</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
@@ -935,15 +938,21 @@
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="B25" s="4">
+        <v>44623</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="D26" s="7"/>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
start to design neural network
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi.borriello2\Desktop\Tirocinio\Tiny-MachineLearning\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E04979-2BBF-41BA-AFCA-7FD5BE5502BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2D7893-0C30-4042-9A36-A01E3683B6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4369CB72-3CB2-48AE-831B-B67D7B2D2361}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Data</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Check conflitto librerie</t>
+  </si>
+  <si>
+    <t>studio ML e reti neurali</t>
   </si>
 </sst>
 </file>
@@ -633,7 +636,7 @@
   <dimension ref="B1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -647,7 +650,7 @@
     <row r="1" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C1" s="6">
         <f>C3+C4+C5+C6+C7+C8+C9+C11+C10+C12+C13+C14+C15+C16+C18+C17+C19+C20++Tabella2[[#Totals],[Ore]]+C22+C23+C24+C25+C26+C176+C28+C177+C21+C29+C27+C30+C31+C32+C33+A35</f>
-        <v>85.5</v>
+        <v>88.5</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
@@ -1018,10 +1021,18 @@
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B30" s="12"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="7"/>
+      <c r="B30" s="12">
+        <v>44632</v>
+      </c>
+      <c r="C30" s="3">
+        <v>3</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="12"/>

</xml_diff>

<commit_message>
add NN to all the tasks
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi.borriello2\Desktop\Tirocinio\Tiny-MachineLearning\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE496149-CED1-4F7D-85C7-47C77ED47FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4278A57A-3DDC-4C7D-8C7A-1CE9AE03ACC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4369CB72-3CB2-48AE-831B-B67D7B2D2361}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10960" xr2:uid="{4369CB72-3CB2-48AE-831B-B67D7B2D2361}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Data</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>grid search e NN in color</t>
+  </si>
+  <si>
+    <t>Grid search finita</t>
+  </si>
+  <si>
+    <t>Tuning NN Frequency</t>
+  </si>
+  <si>
+    <t>Tuning NN color</t>
   </si>
 </sst>
 </file>
@@ -653,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC1F251-2E00-4C93-80E5-7B7C0B1560BE}">
   <dimension ref="B1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +676,7 @@
     <row r="1" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C1" s="6">
         <f>SUM(C3:C56)</f>
-        <v>101</v>
+        <v>106.5</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
@@ -1130,21 +1139,39 @@
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="12"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
+      <c r="B37" s="12">
+        <v>44654</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="E37" s="7"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="12"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+      <c r="B38" s="12">
+        <v>44657</v>
+      </c>
+      <c r="C38" s="3">
+        <v>2</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="E38" s="7"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="12"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
+      <c r="B39" s="12">
+        <v>44658</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="E39" s="7"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding NN in all tasks and Crossval in NN-Keyword
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi.borriello2\Desktop\Tirocinio\Tiny-MachineLearning\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4278A57A-3DDC-4C7D-8C7A-1CE9AE03ACC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B41D44-FD6B-48B7-8540-9AF0AF55FAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10960" xr2:uid="{4369CB72-3CB2-48AE-831B-B67D7B2D2361}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="10780" xr2:uid="{4369CB72-3CB2-48AE-831B-B67D7B2D2361}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>Data</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Tuning NN color</t>
+  </si>
+  <si>
+    <t>Cross Validation NN e creazione NN negli altri task</t>
   </si>
 </sst>
 </file>
@@ -662,24 +665,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC1F251-2E00-4C93-80E5-7B7C0B1560BE}">
   <dimension ref="B1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="64.85546875" customWidth="1"/>
-    <col min="5" max="5" width="56.28515625" customWidth="1"/>
+    <col min="2" max="3" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="64.81640625" customWidth="1"/>
+    <col min="5" max="5" width="56.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C1" s="6">
         <f>SUM(C3:C56)</f>
-        <v>106.5</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+        <v>108.5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -693,7 +696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="4">
         <v>44596</v>
       </c>
@@ -707,7 +710,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="4">
         <v>44597</v>
       </c>
@@ -722,7 +725,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="4">
         <v>44599</v>
       </c>
@@ -736,7 +739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="4">
         <v>44600</v>
       </c>
@@ -751,7 +754,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
         <v>44601</v>
       </c>
@@ -765,7 +768,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
         <v>44602</v>
       </c>
@@ -778,7 +781,7 @@
       <c r="E8" s="3"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
         <v>44603</v>
       </c>
@@ -792,7 +795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>44604</v>
       </c>
@@ -806,7 +809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <v>44605</v>
       </c>
@@ -820,7 +823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
         <v>44607</v>
       </c>
@@ -834,7 +837,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="4">
         <v>44608</v>
       </c>
@@ -848,7 +851,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
         <v>44609</v>
       </c>
@@ -860,7 +863,7 @@
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="4">
         <v>44611</v>
       </c>
@@ -872,7 +875,7 @@
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
         <v>44612</v>
       </c>
@@ -884,7 +887,7 @@
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="4">
         <v>44613</v>
       </c>
@@ -896,7 +899,7 @@
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="4">
         <v>44614</v>
       </c>
@@ -908,7 +911,7 @@
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="4">
         <v>44615</v>
       </c>
@@ -920,7 +923,7 @@
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="4">
         <v>44616</v>
       </c>
@@ -934,7 +937,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="4">
         <v>44618</v>
       </c>
@@ -948,7 +951,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="4">
         <v>44619</v>
       </c>
@@ -960,7 +963,7 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="4">
         <v>44620</v>
       </c>
@@ -972,7 +975,7 @@
       </c>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="4">
         <v>44622</v>
       </c>
@@ -984,7 +987,7 @@
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="4">
         <v>44623</v>
       </c>
@@ -996,7 +999,7 @@
       </c>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="4">
         <v>44626</v>
       </c>
@@ -1008,7 +1011,7 @@
       </c>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="4">
         <v>44627</v>
       </c>
@@ -1020,7 +1023,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="12">
         <v>44629</v>
       </c>
@@ -1032,7 +1035,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="12">
         <v>44630</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="12">
         <v>44632</v>
       </c>
@@ -1060,7 +1063,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="12">
         <v>44633</v>
       </c>
@@ -1072,7 +1075,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="12">
         <v>44634</v>
       </c>
@@ -1086,7 +1089,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="12">
         <v>44635</v>
       </c>
@@ -1098,7 +1101,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="12">
         <v>44643</v>
       </c>
@@ -1110,7 +1113,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" s="12">
         <v>44649</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="12">
         <v>44650</v>
       </c>
@@ -1138,7 +1141,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" s="12">
         <v>44654</v>
       </c>
@@ -1150,7 +1153,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" s="12">
         <v>44657</v>
       </c>
@@ -1162,7 +1165,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" s="12">
         <v>44658</v>
       </c>
@@ -1174,817 +1177,823 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="12"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B40" s="12">
+        <v>44664</v>
+      </c>
+      <c r="C40" s="3">
+        <v>2</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="12"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B42" s="12"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B43" s="12"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B44" s="12"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B45" s="12"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B46" s="12"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B47" s="12"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B48" s="12"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B49" s="12"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B50" s="12"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B51" s="12"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B52" s="12"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B53" s="12"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B54" s="12"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B55" s="12"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B56" s="12"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B57" s="12"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B58" s="12"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B59" s="12"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B60" s="12"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B61" s="12"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B62" s="12"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B63" s="12"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B64" s="12"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B65" s="12"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B66" s="12"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B67" s="12"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B68" s="12"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B69" s="12"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B70" s="12"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B71" s="12"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B72" s="12"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B73" s="12"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B74" s="12"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B75" s="12"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B76" s="12"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B77" s="12"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B78" s="12"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B79" s="12"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B80" s="12"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B81" s="12"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B82" s="12"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B83" s="12"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B84" s="12"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B85" s="12"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B86" s="12"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B87" s="12"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B88" s="12"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B89" s="12"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B90" s="12"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B91" s="12"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B92" s="12"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B93" s="12"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B94" s="12"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B95" s="12"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B96" s="12"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B97" s="12"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B98" s="12"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B99" s="12"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B100" s="12"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B101" s="12"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B102" s="12"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B103" s="12"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B104" s="12"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B105" s="12"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B106" s="12"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B107" s="12"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B108" s="12"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B109" s="12"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B110" s="12"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B111" s="12"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B112" s="12"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B113" s="12"/>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B114" s="12"/>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B115" s="12"/>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B116" s="12"/>
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B117" s="12"/>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B118" s="12"/>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B119" s="12"/>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B120" s="12"/>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B121" s="12"/>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B122" s="12"/>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B123" s="12"/>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B124" s="12"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B125" s="12"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B126" s="12"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B127" s="12"/>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B128" s="12"/>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B129" s="12"/>
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B130" s="12"/>
       <c r="C130" s="3"/>
       <c r="D130" s="3"/>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B131" s="12"/>
       <c r="C131" s="3"/>
       <c r="D131" s="3"/>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B132" s="12"/>
       <c r="C132" s="3"/>
       <c r="D132" s="3"/>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B133" s="12"/>
       <c r="C133" s="3"/>
       <c r="D133" s="3"/>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B134" s="12"/>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B135" s="12"/>
       <c r="C135" s="3"/>
       <c r="D135" s="3"/>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B136" s="12"/>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B137" s="12"/>
       <c r="C137" s="3"/>
       <c r="D137" s="3"/>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B138" s="12"/>
       <c r="C138" s="3"/>
       <c r="D138" s="3"/>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B139" s="12"/>
       <c r="C139" s="3"/>
       <c r="D139" s="3"/>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B140" s="12"/>
       <c r="C140" s="3"/>
       <c r="D140" s="3"/>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B141" s="12"/>
       <c r="C141" s="3"/>
       <c r="D141" s="3"/>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B142" s="12"/>
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B143" s="12"/>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B144" s="12"/>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B145" s="12"/>
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B146" s="12"/>
       <c r="C146" s="3"/>
       <c r="D146" s="3"/>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B147" s="12"/>
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B148" s="12"/>
       <c r="C148" s="3"/>
       <c r="D148" s="3"/>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B149" s="12"/>
       <c r="C149" s="3"/>
       <c r="D149" s="3"/>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B150" s="12"/>
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B151" s="12"/>
       <c r="C151" s="3"/>
       <c r="D151" s="3"/>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B152" s="12"/>
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B153" s="12"/>
       <c r="C153" s="3"/>
       <c r="D153" s="3"/>
       <c r="E153" s="7"/>
     </row>
-    <row r="154" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B154" s="12"/>
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B155" s="12"/>
       <c r="C155" s="3"/>
       <c r="D155" s="3"/>
       <c r="E155" s="7"/>
     </row>
-    <row r="156" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B156" s="12"/>
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
       <c r="E156" s="7"/>
     </row>
-    <row r="157" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B157" s="12"/>
       <c r="C157" s="3"/>
       <c r="D157" s="3"/>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B158" s="12"/>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
       <c r="E158" s="7"/>
     </row>
-    <row r="159" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B159" s="12"/>
       <c r="C159" s="3"/>
       <c r="D159" s="3"/>
       <c r="E159" s="7"/>
     </row>
-    <row r="160" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B160" s="12"/>
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
       <c r="E160" s="7"/>
     </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B161" s="12"/>
       <c r="C161" s="3"/>
       <c r="D161" s="3"/>
       <c r="E161" s="7"/>
     </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B162" s="12"/>
       <c r="C162" s="3"/>
       <c r="D162" s="3"/>
       <c r="E162" s="7"/>
     </row>
-    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B163" s="12"/>
       <c r="C163" s="3"/>
       <c r="D163" s="3"/>
       <c r="E163" s="7"/>
     </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B164" s="12"/>
       <c r="C164" s="3"/>
       <c r="D164" s="3"/>
       <c r="E164" s="7"/>
     </row>
-    <row r="165" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B165" s="12"/>
       <c r="C165" s="3"/>
       <c r="D165" s="3"/>
       <c r="E165" s="7"/>
     </row>
-    <row r="166" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B166" s="12"/>
       <c r="C166" s="3"/>
       <c r="D166" s="3"/>
       <c r="E166" s="7"/>
     </row>
-    <row r="167" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B167" s="12"/>
       <c r="C167" s="3"/>
       <c r="D167" s="3"/>
       <c r="E167" s="7"/>
     </row>
-    <row r="168" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B168" s="12"/>
       <c r="C168" s="3"/>
       <c r="D168" s="3"/>
       <c r="E168" s="7"/>
     </row>
-    <row r="169" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B169" s="12"/>
       <c r="C169" s="3"/>
       <c r="D169" s="3"/>
       <c r="E169" s="7"/>
     </row>
-    <row r="170" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B170" s="12"/>
       <c r="C170" s="3"/>
       <c r="D170" s="3"/>
       <c r="E170" s="7"/>
     </row>
-    <row r="171" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B171" s="12"/>
       <c r="C171" s="3"/>
       <c r="D171" s="3"/>
       <c r="E171" s="7"/>
     </row>
-    <row r="172" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B172" s="12"/>
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
       <c r="E172" s="7"/>
     </row>
-    <row r="173" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B173" s="12"/>
       <c r="C173" s="3"/>
       <c r="D173" s="3"/>
       <c r="E173" s="7"/>
     </row>
-    <row r="174" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B174" s="12"/>
       <c r="C174" s="3"/>
       <c r="D174" s="3"/>
       <c r="E174" s="7"/>
     </row>
-    <row r="175" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B175" s="3"/>
       <c r="D175" s="3"/>
       <c r="E175" s="3"/>

</xml_diff>

<commit_message>
Reorganize freq and colors tasks
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
   <si>
     <t xml:space="preserve">Data</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t xml:space="preserve">Report Tabelle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ristrutturazione progetto c++</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,7 @@
   </sheetPr>
   <dimension ref="B1:I175"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
     </sheetView>
   </sheetViews>
@@ -533,7 +536,7 @@
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="1" t="n">
         <f aca="false">SUM(C3:C56)</f>
-        <v>128.5</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1103,7 +1106,7 @@
       </c>
       <c r="E45" s="11"/>
     </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="12" t="n">
         <v>44686</v>
       </c>
@@ -1115,10 +1118,16 @@
       </c>
       <c r="E46" s="11"/>
     </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="12"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="12" t="n">
+        <v>44687</v>
+      </c>
+      <c r="C47" s="7" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="E47" s="11"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Try to fix issue with port COM6
</commit_message>
<xml_diff>
--- a/report/Report.xlsx
+++ b/report/Report.xlsx
@@ -1,17 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi.borriello2\Desktop\Tirocinio\Tiny-MachineLearning\report\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F95F6D8-3569-4F6D-8A31-F38DE728B40E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -22,79 +37,79 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
-    <t xml:space="preserve">Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fonti utilizzate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Studio del TinyML / Random For</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pdf prof / Youtube</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SetUp Jupyter e studio arduino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dispense Unibo / Youtube</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test sensori arduino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arduino Doc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Studio ML e esercitazioni</t>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Ore</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Fonti utilizzate</t>
+  </si>
+  <si>
+    <t>Studio del TinyML / Random For</t>
+  </si>
+  <si>
+    <t>Pdf prof / Youtube</t>
+  </si>
+  <si>
+    <t>SetUp Jupyter e studio arduino</t>
+  </si>
+  <si>
+    <t>Dispense Unibo / Youtube</t>
+  </si>
+  <si>
+    <t>Test sensori arduino</t>
+  </si>
+  <si>
+    <t>Arduino Doc</t>
+  </si>
+  <si>
+    <t>Studio ML e esercitazioni</t>
   </si>
   <si>
     <t xml:space="preserve">Youtube </t>
   </si>
   <si>
-    <t xml:space="preserve">Studio Jupyter e dispense prof</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Studio modelli alternativi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sklearn doc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementazione algo altern</t>
+    <t>Studio Jupyter e dispense prof</t>
+  </si>
+  <si>
+    <t>Studio modelli alternativi</t>
+  </si>
+  <si>
+    <t>Sklearn doc</t>
+  </si>
+  <si>
+    <t>Implementazione algo altern</t>
   </si>
   <si>
     <t xml:space="preserve">Studio XGB </t>
   </si>
   <si>
-    <t xml:space="preserve">Meeting &amp; Studio m2cgen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Github</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cross Validation e Model Compar.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model C. e test dei modelli su AD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Studio memoria e Inferenza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test vari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">studio elettronica arduino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test perf su ard</t>
+    <t>Meeting &amp; Studio m2cgen</t>
+  </si>
+  <si>
+    <t>Github</t>
+  </si>
+  <si>
+    <t>Cross Validation e Model Compar.</t>
+  </si>
+  <si>
+    <t>Model C. e test dei modelli su AD</t>
+  </si>
+  <si>
+    <t>Studio memoria e Inferenza</t>
+  </si>
+  <si>
+    <t>test vari</t>
+  </si>
+  <si>
+    <t>studio elettronica arduino</t>
+  </si>
+  <si>
+    <t>test perf su ard</t>
   </si>
   <si>
     <t xml:space="preserve">Ricerca Paper </t>
@@ -103,110 +118,108 @@
     <t xml:space="preserve">Google Scholar / </t>
   </si>
   <si>
-    <t xml:space="preserve">BenchMarking Freq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arduino Studio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start keyword-spotting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Report modelli su arduino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test raddoppiando valori</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call e check librerie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raccolta campioni e test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check conflitto librerie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fix librerie conflitto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Studio ML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corso ML magistrale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">studio ML e reti neurali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementazione Rete neurale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test su arduino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EloquentDoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call e Tuning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grid Search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grid search e NN in color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grid search finita</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tuning NN Frequency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tuning NN color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cross Validation NN e creazione NN negli altri task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15-apr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meeting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16-apr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fix Cross-val e valutazione Test set altri task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Record nuovi valori e test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Importazione rete su arduino e scrittura file arduino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valutazione Test set su arduino e call</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Report Tabelle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ristrutturazione progetto c++</t>
+    <t>BenchMarking Freq</t>
+  </si>
+  <si>
+    <t>Arduino Studio</t>
+  </si>
+  <si>
+    <t>Start keyword-spotting</t>
+  </si>
+  <si>
+    <t>Report modelli su arduino</t>
+  </si>
+  <si>
+    <t>Test raddoppiando valori</t>
+  </si>
+  <si>
+    <t>Call e check librerie</t>
+  </si>
+  <si>
+    <t>Raccolta campioni e test</t>
+  </si>
+  <si>
+    <t>Check conflitto librerie</t>
+  </si>
+  <si>
+    <t>Fix librerie conflitto</t>
+  </si>
+  <si>
+    <t>Studio ML</t>
+  </si>
+  <si>
+    <t>Corso ML magistrale</t>
+  </si>
+  <si>
+    <t>studio ML e reti neurali</t>
+  </si>
+  <si>
+    <t>Implementazione Rete neurale</t>
+  </si>
+  <si>
+    <t>Test su arduino</t>
+  </si>
+  <si>
+    <t>EloquentDoc</t>
+  </si>
+  <si>
+    <t>Call e Tuning</t>
+  </si>
+  <si>
+    <t>grid Search</t>
+  </si>
+  <si>
+    <t>grid search e NN in color</t>
+  </si>
+  <si>
+    <t>Grid search finita</t>
+  </si>
+  <si>
+    <t>Tuning NN Frequency</t>
+  </si>
+  <si>
+    <t>Tuning NN color</t>
+  </si>
+  <si>
+    <t>Cross Validation NN e creazione NN negli altri task</t>
+  </si>
+  <si>
+    <t>15-apr</t>
+  </si>
+  <si>
+    <t>meeting</t>
+  </si>
+  <si>
+    <t>16-apr</t>
+  </si>
+  <si>
+    <t>Fix Cross-val e valutazione Test set altri task</t>
+  </si>
+  <si>
+    <t>Record nuovi valori e test</t>
+  </si>
+  <si>
+    <t>Importazione rete su arduino e scrittura file arduino</t>
+  </si>
+  <si>
+    <t>Valutazione Test set su arduino e call</t>
+  </si>
+  <si>
+    <t>Report Tabelle</t>
+  </si>
+  <si>
+    <t>Ristrutturazione progetto c++</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="167" formatCode="d\-mmm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -215,22 +228,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -245,7 +243,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -286,160 +284,78 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="double"/>
-      <bottom style="thin"/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="3">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF70AD47"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC3C7D1"/>
-          <bgColor rgb="FF181B28"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF4472C4"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -498,48 +414,357 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella2" displayName="Tabella2" ref="B2:E175" headerRowCount="1" totalsRowCount="1" totalsRowShown="1">
-  <autoFilter ref="B2:E175"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella2" displayName="Tabella2" ref="B2:E175" totalsRowCount="1">
+  <autoFilter ref="B2:E174" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Data"/>
-    <tableColumn id="2" name="Ore"/>
-    <tableColumn id="3" name="Task"/>
-    <tableColumn id="4" name="Fonti utilizzate"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Data" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ore"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Task" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Fonti utilizzate" totalsRowDxfId="0"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I175"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C59" activeCellId="0" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="64.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="56.27"/>
+    <col min="2" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="64.85546875" customWidth="1"/>
+    <col min="5" max="5" width="56.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="1" t="n">
-        <f aca="false">SUM(C3:C56)</f>
-        <v>131.5</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C1" s="1">
+        <f>SUM(C3:C56)</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -553,11 +778,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="6" t="n">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
         <v>44596</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="7">
         <v>4</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -567,11 +792,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="6" t="n">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
         <v>44597</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="7">
         <v>3</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -582,11 +807,11 @@
       </c>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6" t="n">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
         <v>44599</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="7">
         <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -596,11 +821,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6" t="n">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
         <v>44600</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="7">
         <v>5</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -611,11 +836,11 @@
       </c>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6" t="n">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
         <v>44601</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="7">
         <v>6</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -625,11 +850,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6" t="n">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
         <v>44602</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="7">
         <v>4</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -638,11 +863,11 @@
       <c r="E8" s="7"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6" t="n">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
         <v>44603</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="7">
         <v>3</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -652,11 +877,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6" t="n">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
         <v>44604</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="7">
         <v>2.5</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -666,11 +891,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="n">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
         <v>44605</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="7">
         <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -680,11 +905,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="n">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
         <v>44607</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C12" s="7">
         <v>3</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -694,11 +919,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="6" t="n">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
         <v>44608</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="7">
         <v>5</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -708,11 +933,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="6" t="n">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
         <v>44609</v>
       </c>
-      <c r="C14" s="7" t="n">
+      <c r="C14" s="7">
         <v>4.5</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -720,11 +945,11 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="6" t="n">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
         <v>44611</v>
       </c>
-      <c r="C15" s="7" t="n">
+      <c r="C15" s="7">
         <v>6</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -732,11 +957,11 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="6" t="n">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
         <v>44612</v>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="7">
         <v>2</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -744,11 +969,11 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="6" t="n">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
         <v>44613</v>
       </c>
-      <c r="C17" s="7" t="n">
+      <c r="C17" s="7">
         <v>2</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -756,11 +981,11 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="6" t="n">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
         <v>44614</v>
       </c>
-      <c r="C18" s="7" t="n">
+      <c r="C18" s="7">
         <v>1.5</v>
       </c>
       <c r="D18" s="7" t="s">
@@ -768,11 +993,11 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="6" t="n">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
         <v>44615</v>
       </c>
-      <c r="C19" s="7" t="n">
+      <c r="C19" s="7">
         <v>1.5</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -780,11 +1005,11 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="6" t="n">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
         <v>44616</v>
       </c>
-      <c r="C20" s="7" t="n">
+      <c r="C20" s="7">
         <v>2</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -794,11 +1019,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="6" t="n">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
         <v>44618</v>
       </c>
-      <c r="C21" s="7" t="n">
+      <c r="C21" s="7">
         <v>3.5</v>
       </c>
       <c r="D21" s="7" t="s">
@@ -808,11 +1033,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="6" t="n">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
         <v>44619</v>
       </c>
-      <c r="C22" s="7" t="n">
+      <c r="C22" s="7">
         <v>5</v>
       </c>
       <c r="D22" s="7" t="s">
@@ -820,11 +1045,11 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="6" t="n">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
         <v>44620</v>
       </c>
-      <c r="C23" s="11" t="n">
+      <c r="C23" s="11">
         <v>3</v>
       </c>
       <c r="D23" s="7" t="s">
@@ -832,11 +1057,11 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="6" t="n">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
         <v>44622</v>
       </c>
-      <c r="C24" s="7" t="n">
+      <c r="C24" s="7">
         <v>2</v>
       </c>
       <c r="D24" s="7" t="s">
@@ -844,11 +1069,11 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="6" t="n">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
         <v>44623</v>
       </c>
-      <c r="C25" s="7" t="n">
+      <c r="C25" s="7">
         <v>2</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -856,11 +1081,11 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="6" t="n">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="6">
         <v>44626</v>
       </c>
-      <c r="C26" s="7" t="n">
+      <c r="C26" s="7">
         <v>4</v>
       </c>
       <c r="D26" s="7" t="s">
@@ -868,11 +1093,11 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="6" t="n">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
         <v>44627</v>
       </c>
-      <c r="C27" s="7" t="n">
+      <c r="C27" s="7">
         <v>2</v>
       </c>
       <c r="D27" s="7" t="s">
@@ -880,11 +1105,11 @@
       </c>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="12" t="n">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="12">
         <v>44629</v>
       </c>
-      <c r="C28" s="7" t="n">
+      <c r="C28" s="7">
         <v>1</v>
       </c>
       <c r="D28" s="7" t="s">
@@ -892,11 +1117,11 @@
       </c>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="12" t="n">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="12">
         <v>44630</v>
       </c>
-      <c r="C29" s="7" t="n">
+      <c r="C29" s="7">
         <v>3</v>
       </c>
       <c r="D29" s="7" t="s">
@@ -906,11 +1131,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="12" t="n">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="12">
         <v>44632</v>
       </c>
-      <c r="C30" s="7" t="n">
+      <c r="C30" s="7">
         <v>3</v>
       </c>
       <c r="D30" s="7" t="s">
@@ -920,11 +1145,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="12" t="n">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="12">
         <v>44633</v>
       </c>
-      <c r="C31" s="7" t="n">
+      <c r="C31" s="7">
         <v>4.5</v>
       </c>
       <c r="D31" s="7" t="s">
@@ -932,11 +1157,11 @@
       </c>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="12" t="n">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="12">
         <v>44634</v>
       </c>
-      <c r="C32" s="7" t="n">
+      <c r="C32" s="7">
         <v>2</v>
       </c>
       <c r="D32" s="7" t="s">
@@ -946,11 +1171,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="12" t="n">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="12">
         <v>44635</v>
       </c>
-      <c r="C33" s="7" t="n">
+      <c r="C33" s="7">
         <v>1</v>
       </c>
       <c r="D33" s="7" t="s">
@@ -958,11 +1183,11 @@
       </c>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="12" t="n">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="12">
         <v>44643</v>
       </c>
-      <c r="C34" s="7" t="n">
+      <c r="C34" s="7">
         <v>2</v>
       </c>
       <c r="D34" s="7" t="s">
@@ -970,11 +1195,11 @@
       </c>
       <c r="E34" s="11"/>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="12" t="n">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="12">
         <v>44649</v>
       </c>
-      <c r="C35" s="7" t="n">
+      <c r="C35" s="7">
         <v>1</v>
       </c>
       <c r="D35" s="7" t="s">
@@ -984,11 +1209,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="12" t="n">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="12">
         <v>44650</v>
       </c>
-      <c r="C36" s="7" t="n">
+      <c r="C36" s="7">
         <v>2</v>
       </c>
       <c r="D36" s="7" t="s">
@@ -998,11 +1223,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="12" t="n">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="12">
         <v>44654</v>
       </c>
-      <c r="C37" s="7" t="n">
+      <c r="C37" s="7">
         <v>2</v>
       </c>
       <c r="D37" s="7" t="s">
@@ -1010,11 +1235,11 @@
       </c>
       <c r="E37" s="11"/>
     </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="12" t="n">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="12">
         <v>44657</v>
       </c>
-      <c r="C38" s="7" t="n">
+      <c r="C38" s="7">
         <v>2</v>
       </c>
       <c r="D38" s="7" t="s">
@@ -1022,11 +1247,11 @@
       </c>
       <c r="E38" s="11"/>
     </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="12" t="n">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="12">
         <v>44658</v>
       </c>
-      <c r="C39" s="7" t="n">
+      <c r="C39" s="7">
         <v>1.5</v>
       </c>
       <c r="D39" s="7" t="s">
@@ -1034,11 +1259,11 @@
       </c>
       <c r="E39" s="11"/>
     </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="12" t="n">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="12">
         <v>44664</v>
       </c>
-      <c r="C40" s="7" t="n">
+      <c r="C40" s="7">
         <v>2</v>
       </c>
       <c r="D40" s="7" t="s">
@@ -1046,11 +1271,11 @@
       </c>
       <c r="E40" s="11"/>
     </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="7" t="n">
+      <c r="C41" s="7">
         <v>1</v>
       </c>
       <c r="D41" s="7" t="s">
@@ -1058,11 +1283,11 @@
       </c>
       <c r="E41" s="11"/>
     </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="7" t="n">
+      <c r="C42" s="7">
         <v>3</v>
       </c>
       <c r="D42" s="7" t="s">
@@ -1070,11 +1295,11 @@
       </c>
       <c r="E42" s="11"/>
     </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="12" t="n">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="12">
         <v>44674</v>
       </c>
-      <c r="C43" s="7" t="n">
+      <c r="C43" s="7">
         <v>3</v>
       </c>
       <c r="D43" s="7" t="s">
@@ -1082,11 +1307,11 @@
       </c>
       <c r="E43" s="11"/>
     </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="12" t="n">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="12">
         <v>44675</v>
       </c>
-      <c r="C44" s="7" t="n">
+      <c r="C44" s="7">
         <v>4</v>
       </c>
       <c r="D44" s="7" t="s">
@@ -1094,11 +1319,11 @@
       </c>
       <c r="E44" s="11"/>
     </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="12" t="n">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="12">
         <v>44678</v>
       </c>
-      <c r="C45" s="7" t="n">
+      <c r="C45" s="7">
         <v>2.5</v>
       </c>
       <c r="D45" s="7" t="s">
@@ -1106,11 +1331,11 @@
       </c>
       <c r="E45" s="11"/>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="12" t="n">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="12">
         <v>44686</v>
       </c>
-      <c r="C46" s="7" t="n">
+      <c r="C46" s="7">
         <v>6.5</v>
       </c>
       <c r="D46" s="7" t="s">
@@ -1118,11 +1343,11 @@
       </c>
       <c r="E46" s="11"/>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="12" t="n">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="12">
         <v>44687</v>
       </c>
-      <c r="C47" s="7" t="n">
+      <c r="C47" s="7">
         <v>1.5</v>
       </c>
       <c r="D47" s="7" t="s">
@@ -1130,788 +1355,783 @@
       </c>
       <c r="E47" s="11"/>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="12" t="n">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="12">
         <v>44688</v>
       </c>
-      <c r="C48" s="7" t="n">
-        <v>1.5</v>
+      <c r="C48" s="7">
+        <v>5</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>57</v>
       </c>
       <c r="E48" s="11"/>
     </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="12"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="11"/>
     </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="12"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="11"/>
     </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="12"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="11"/>
     </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="12"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="11"/>
     </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="12"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="11"/>
     </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="12"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="11"/>
     </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="12"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="11"/>
     </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="12"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="11"/>
     </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="12"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="11"/>
     </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="12"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="11"/>
     </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="12"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="11"/>
     </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="12"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="11"/>
     </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="12"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="11"/>
     </row>
-    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="12"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="11"/>
     </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="12"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="11"/>
     </row>
-    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="12"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="11"/>
     </row>
-    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="12"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="11"/>
     </row>
-    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="12"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="11"/>
     </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="12"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="11"/>
     </row>
-    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="12"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
       <c r="E68" s="11"/>
     </row>
-    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="12"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
       <c r="E69" s="11"/>
     </row>
-    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="12"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="11"/>
     </row>
-    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="12"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="11"/>
     </row>
-    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="12"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="11"/>
     </row>
-    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="12"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" s="11"/>
     </row>
-    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="12"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
       <c r="E74" s="11"/>
     </row>
-    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="12"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="11"/>
     </row>
-    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="12"/>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="11"/>
     </row>
-    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="12"/>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="11"/>
     </row>
-    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" s="12"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="11"/>
     </row>
-    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" s="12"/>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="11"/>
     </row>
-    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="12"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="11"/>
     </row>
-    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="12"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="11"/>
     </row>
-    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="12"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
       <c r="E82" s="11"/>
     </row>
-    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="12"/>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="11"/>
     </row>
-    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="12"/>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="11"/>
     </row>
-    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="12"/>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="11"/>
     </row>
-    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="12"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="11"/>
     </row>
-    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="12"/>
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="11"/>
     </row>
-    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="12"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="11"/>
     </row>
-    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="12"/>
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
       <c r="E89" s="11"/>
     </row>
-    <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="12"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="11"/>
     </row>
-    <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="12"/>
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
       <c r="E91" s="11"/>
     </row>
-    <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="12"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
       <c r="E92" s="11"/>
     </row>
-    <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="12"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
       <c r="E93" s="11"/>
     </row>
-    <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="12"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
       <c r="E94" s="11"/>
     </row>
-    <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="12"/>
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
       <c r="E95" s="11"/>
     </row>
-    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="12"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
       <c r="E96" s="11"/>
     </row>
-    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" s="12"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
       <c r="E97" s="11"/>
     </row>
-    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="12"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
       <c r="E98" s="11"/>
     </row>
-    <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99" s="12"/>
       <c r="C99" s="7"/>
       <c r="D99" s="7"/>
       <c r="E99" s="11"/>
     </row>
-    <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B100" s="12"/>
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
       <c r="E100" s="11"/>
     </row>
-    <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B101" s="12"/>
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
       <c r="E101" s="11"/>
     </row>
-    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B102" s="12"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
       <c r="E102" s="11"/>
     </row>
-    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B103" s="12"/>
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
       <c r="E103" s="11"/>
     </row>
-    <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B104" s="12"/>
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="11"/>
     </row>
-    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B105" s="12"/>
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="11"/>
     </row>
-    <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B106" s="12"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="11"/>
     </row>
-    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B107" s="12"/>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="11"/>
     </row>
-    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B108" s="12"/>
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="11"/>
     </row>
-    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B109" s="12"/>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="11"/>
     </row>
-    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B110" s="12"/>
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="11"/>
     </row>
-    <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B111" s="12"/>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="11"/>
     </row>
-    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B112" s="12"/>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="11"/>
     </row>
-    <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113" s="12"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="11"/>
     </row>
-    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B114" s="12"/>
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
       <c r="E114" s="11"/>
     </row>
-    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B115" s="12"/>
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
       <c r="E115" s="11"/>
     </row>
-    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B116" s="12"/>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="11"/>
     </row>
-    <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B117" s="12"/>
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="11"/>
     </row>
-    <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B118" s="12"/>
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
       <c r="E118" s="11"/>
     </row>
-    <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B119" s="12"/>
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
       <c r="E119" s="11"/>
     </row>
-    <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B120" s="12"/>
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
       <c r="E120" s="11"/>
     </row>
-    <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B121" s="12"/>
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="11"/>
     </row>
-    <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B122" s="12"/>
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
       <c r="E122" s="11"/>
     </row>
-    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B123" s="12"/>
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
       <c r="E123" s="11"/>
     </row>
-    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B124" s="12"/>
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="11"/>
     </row>
-    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B125" s="12"/>
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
       <c r="E125" s="11"/>
     </row>
-    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B126" s="12"/>
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
       <c r="E126" s="11"/>
     </row>
-    <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B127" s="12"/>
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
       <c r="E127" s="11"/>
     </row>
-    <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B128" s="12"/>
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
       <c r="E128" s="11"/>
     </row>
-    <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B129" s="12"/>
       <c r="C129" s="7"/>
       <c r="D129" s="7"/>
       <c r="E129" s="11"/>
     </row>
-    <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B130" s="12"/>
       <c r="C130" s="7"/>
       <c r="D130" s="7"/>
       <c r="E130" s="11"/>
     </row>
-    <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B131" s="12"/>
       <c r="C131" s="7"/>
       <c r="D131" s="7"/>
       <c r="E131" s="11"/>
     </row>
-    <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B132" s="12"/>
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
       <c r="E132" s="11"/>
     </row>
-    <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B133" s="12"/>
       <c r="C133" s="7"/>
       <c r="D133" s="7"/>
       <c r="E133" s="11"/>
     </row>
-    <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B134" s="12"/>
       <c r="C134" s="7"/>
       <c r="D134" s="7"/>
       <c r="E134" s="11"/>
     </row>
-    <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B135" s="12"/>
       <c r="C135" s="7"/>
       <c r="D135" s="7"/>
       <c r="E135" s="11"/>
     </row>
-    <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B136" s="12"/>
       <c r="C136" s="7"/>
       <c r="D136" s="7"/>
       <c r="E136" s="11"/>
     </row>
-    <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B137" s="12"/>
       <c r="C137" s="7"/>
       <c r="D137" s="7"/>
       <c r="E137" s="11"/>
     </row>
-    <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B138" s="12"/>
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
       <c r="E138" s="11"/>
     </row>
-    <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B139" s="12"/>
       <c r="C139" s="7"/>
       <c r="D139" s="7"/>
       <c r="E139" s="11"/>
     </row>
-    <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B140" s="12"/>
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
       <c r="E140" s="11"/>
     </row>
-    <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B141" s="12"/>
       <c r="C141" s="7"/>
       <c r="D141" s="7"/>
       <c r="E141" s="11"/>
     </row>
-    <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B142" s="12"/>
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
       <c r="E142" s="11"/>
     </row>
-    <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B143" s="12"/>
       <c r="C143" s="7"/>
       <c r="D143" s="7"/>
       <c r="E143" s="11"/>
     </row>
-    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B144" s="12"/>
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
       <c r="E144" s="11"/>
     </row>
-    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B145" s="12"/>
       <c r="C145" s="7"/>
       <c r="D145" s="7"/>
       <c r="E145" s="11"/>
     </row>
-    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B146" s="12"/>
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
       <c r="E146" s="11"/>
     </row>
-    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B147" s="12"/>
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
       <c r="E147" s="11"/>
     </row>
-    <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B148" s="12"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
       <c r="E148" s="11"/>
     </row>
-    <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B149" s="12"/>
       <c r="C149" s="7"/>
       <c r="D149" s="7"/>
       <c r="E149" s="11"/>
     </row>
-    <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B150" s="12"/>
       <c r="C150" s="7"/>
       <c r="D150" s="7"/>
       <c r="E150" s="11"/>
     </row>
-    <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B151" s="12"/>
       <c r="C151" s="7"/>
       <c r="D151" s="7"/>
       <c r="E151" s="11"/>
     </row>
-    <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B152" s="12"/>
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
       <c r="E152" s="11"/>
     </row>
-    <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B153" s="12"/>
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
       <c r="E153" s="11"/>
     </row>
-    <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B154" s="12"/>
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
       <c r="E154" s="11"/>
     </row>
-    <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B155" s="12"/>
       <c r="C155" s="7"/>
       <c r="D155" s="7"/>
       <c r="E155" s="11"/>
     </row>
-    <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B156" s="12"/>
       <c r="C156" s="7"/>
       <c r="D156" s="7"/>
       <c r="E156" s="11"/>
     </row>
-    <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B157" s="12"/>
       <c r="C157" s="7"/>
       <c r="D157" s="7"/>
       <c r="E157" s="11"/>
     </row>
-    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B158" s="12"/>
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>
       <c r="E158" s="11"/>
     </row>
-    <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B159" s="12"/>
       <c r="C159" s="7"/>
       <c r="D159" s="7"/>
       <c r="E159" s="11"/>
     </row>
-    <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B160" s="12"/>
       <c r="C160" s="7"/>
       <c r="D160" s="7"/>
       <c r="E160" s="11"/>
     </row>
-    <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B161" s="12"/>
       <c r="C161" s="7"/>
       <c r="D161" s="7"/>
       <c r="E161" s="11"/>
     </row>
-    <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B162" s="12"/>
       <c r="C162" s="7"/>
       <c r="D162" s="7"/>
       <c r="E162" s="11"/>
     </row>
-    <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B163" s="12"/>
       <c r="C163" s="7"/>
       <c r="D163" s="7"/>
       <c r="E163" s="11"/>
     </row>
-    <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B164" s="12"/>
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
       <c r="E164" s="11"/>
     </row>
-    <row r="165" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B165" s="12"/>
       <c r="C165" s="7"/>
       <c r="D165" s="7"/>
       <c r="E165" s="11"/>
     </row>
-    <row r="166" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B166" s="12"/>
       <c r="C166" s="7"/>
       <c r="D166" s="7"/>
       <c r="E166" s="11"/>
     </row>
-    <row r="167" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B167" s="12"/>
       <c r="C167" s="7"/>
       <c r="D167" s="7"/>
       <c r="E167" s="11"/>
     </row>
-    <row r="168" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B168" s="12"/>
       <c r="C168" s="7"/>
       <c r="D168" s="7"/>
       <c r="E168" s="11"/>
     </row>
-    <row r="169" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B169" s="12"/>
       <c r="C169" s="7"/>
       <c r="D169" s="7"/>
       <c r="E169" s="11"/>
     </row>
-    <row r="170" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B170" s="12"/>
       <c r="C170" s="7"/>
       <c r="D170" s="7"/>
       <c r="E170" s="11"/>
     </row>
-    <row r="171" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B171" s="12"/>
       <c r="C171" s="7"/>
       <c r="D171" s="7"/>
       <c r="E171" s="11"/>
     </row>
-    <row r="172" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B172" s="12"/>
       <c r="C172" s="7"/>
       <c r="D172" s="7"/>
       <c r="E172" s="11"/>
     </row>
-    <row r="173" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B173" s="12"/>
       <c r="C173" s="7"/>
       <c r="D173" s="7"/>
       <c r="E173" s="11"/>
     </row>
-    <row r="174" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B174" s="12"/>
       <c r="C174" s="7"/>
       <c r="D174" s="7"/>
       <c r="E174" s="11"/>
     </row>
-    <row r="175" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B175" s="7"/>
       <c r="D175" s="7"/>
       <c r="E175" s="7"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <tableParts>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>

</xml_diff>